<commit_message>
Initial Excel Document change test
</commit_message>
<xml_diff>
--- a/OA3801_ProjectGradeSheet.xlsx
+++ b/OA3801_ProjectGradeSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossschuchard/Library/CloudStorage/Box-Box/OR_Computation/OA3801/OA3801_WI23_RS/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmbromley/OA3801FinalProject/OA3801FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEBDCAC-30BF-014D-98A3-3CDFF32C5B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D6F9CF-482A-DF4C-94B7-8AA98C8C0F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="760" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student score" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Points Available</t>
   </si>
@@ -333,6 +333,9 @@
       </rPr>
       <t xml:space="preserve">  LastName, FirstName</t>
     </r>
+  </si>
+  <si>
+    <t>Bromley Test</t>
   </si>
 </sst>
 </file>
@@ -975,7 +978,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1200,77 +1203,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1306,6 +1257,78 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1335,27 +1358,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -1722,7 +1724,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="A1:F23"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1738,31 +1740,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="19">
-      <c r="A2" s="113"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="19">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1776,11 +1778,11 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="20" thickBot="1">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="117"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
       <c r="D5" s="54" t="s">
         <v>0</v>
       </c>
@@ -1793,10 +1795,10 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="50" customHeight="1">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="93" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="55" t="s">
@@ -1810,10 +1812,13 @@
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="1"/>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="50" customHeight="1">
-      <c r="A7" s="107"/>
-      <c r="B7" s="110"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="49" t="s">
         <v>7</v>
       </c>
@@ -1827,8 +1832,8 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="50" customHeight="1">
-      <c r="A8" s="107"/>
-      <c r="B8" s="110"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="49" t="s">
         <v>9</v>
       </c>
@@ -1842,8 +1847,8 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="50" customHeight="1">
-      <c r="A9" s="107"/>
-      <c r="B9" s="110"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="49" t="s">
         <v>8</v>
       </c>
@@ -1857,8 +1862,8 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="50" customHeight="1">
-      <c r="A10" s="107"/>
-      <c r="B10" s="110"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="50" t="s">
         <v>10</v>
       </c>
@@ -1874,8 +1879,8 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="50" customHeight="1">
-      <c r="A11" s="107"/>
-      <c r="B11" s="110"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="50" t="s">
         <v>16</v>
       </c>
@@ -1889,8 +1894,8 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="50" customHeight="1" thickBot="1">
-      <c r="A12" s="108"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="60" t="s">
         <v>47</v>
       </c>
@@ -1904,10 +1909,10 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="37" customHeight="1">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="123" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="64" t="s">
@@ -1924,8 +1929,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="37" customHeight="1">
-      <c r="A14" s="83"/>
-      <c r="B14" s="104"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="45" t="s">
         <v>13</v>
       </c>
@@ -1940,8 +1945,8 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="37" customHeight="1">
-      <c r="A15" s="83"/>
-      <c r="B15" s="104"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="47" t="s">
         <v>51</v>
       </c>
@@ -1956,8 +1961,8 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="37" customHeight="1" thickBot="1">
-      <c r="A16" s="84"/>
-      <c r="B16" s="105"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="69" t="s">
         <v>11</v>
       </c>
@@ -1972,10 +1977,10 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="66" customHeight="1">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="123" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="72" t="s">
@@ -1991,62 +1996,62 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1">
-      <c r="A18" s="83"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="98" t="s">
+      <c r="A18" s="103"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="99">
+      <c r="D18" s="119">
         <v>10</v>
       </c>
-      <c r="E18" s="101">
+      <c r="E18" s="121">
         <v>10</v>
       </c>
-      <c r="F18" s="91"/>
+      <c r="F18" s="111"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" thickBot="1">
-      <c r="A19" s="84"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="90"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" ht="23" customHeight="1">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="92">
+      <c r="D20" s="112">
         <v>15</v>
       </c>
-      <c r="E20" s="95">
+      <c r="E20" s="115">
         <v>15</v>
       </c>
-      <c r="F20" s="88"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1">
-      <c r="A21" s="83"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="89"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="109"/>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" ht="56" customHeight="1" thickBot="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="105"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="90"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="110"/>
     </row>
     <row r="23" spans="1:7" ht="19">
       <c r="C23" s="76" t="s">
@@ -2067,12 +2072,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:B12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A13:A16"/>
@@ -2087,6 +2086,12 @@
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" copies="3"/>
@@ -2235,11 +2240,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:10" ht="23" customHeight="1">
       <c r="A2" t="s">
@@ -2248,11 +2253,11 @@
     </row>
     <row r="3" spans="1:10" ht="12" customHeight="1"/>
     <row r="4" spans="1:10" ht="83" customHeight="1">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
@@ -2334,23 +2339,22 @@
       <c r="C15" s="37"/>
     </row>
     <row r="16" spans="1:10" ht="54" customHeight="1">
-      <c r="A16" s="128" t="s">
+      <c r="A16" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="130"/>
-      <c r="C16" s="129"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="83"/>
     </row>
     <row r="17" spans="1:3" ht="17" customHeight="1">
-      <c r="A17" s="134"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="136"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="131" t="s">
+      <c r="A18" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="132"/>
-      <c r="C18" s="133"/>
+      <c r="C18" s="86"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="43" t="s">
@@ -2429,53 +2433,53 @@
       <c r="C28" s="34"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="121"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="129"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="122" t="s">
+      <c r="A31" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="123"/>
-      <c r="C31" s="124"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="132"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="122"/>
-      <c r="B32" s="123"/>
-      <c r="C32" s="124"/>
+      <c r="A32" s="130"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="132"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="122"/>
-      <c r="B33" s="123"/>
-      <c r="C33" s="124"/>
+      <c r="A33" s="130"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="132"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="122"/>
-      <c r="B34" s="123"/>
-      <c r="C34" s="124"/>
+      <c r="A34" s="130"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="132"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="122"/>
-      <c r="B35" s="123"/>
-      <c r="C35" s="124"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="132"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="122"/>
-      <c r="B36" s="123"/>
-      <c r="C36" s="124"/>
+      <c r="A36" s="130"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="132"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="122"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="124"/>
+      <c r="A37" s="130"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="132"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="125"/>
-      <c r="B38" s="126"/>
-      <c r="C38" s="127"/>
+      <c r="A38" s="133"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>